<commit_message>
Test run complete, bugfixes needed
</commit_message>
<xml_diff>
--- a/Graphs/normal flow rate details.xlsx
+++ b/Graphs/normal flow rate details.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="513" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="646" uniqueCount="15">
   <si>
     <t>normal_flow_rate_details1</t>
   </si>
@@ -109,9 +109,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="true"/>
-    <col min="2" max="2" width="13.46484375" customWidth="true"/>
-    <col min="3" max="3" width="4.73046875" customWidth="true"/>
+    <col min="1" max="1" width="26.42578125" customWidth="true"/>
+    <col min="2" max="2" width="14.5703125" customWidth="true"/>
+    <col min="3" max="3" width="4.85546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -130,7 +130,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>49.144947897927672</v>
+        <v>54.473378555443993</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>11</v>
@@ -141,7 +141,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>33.128717724147037</v>
+        <v>32.598269851519511</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>11</v>
@@ -152,7 +152,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>10.503584335380593</v>
+        <v>13.411851961272751</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
@@ -163,7 +163,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>26.962458710109107</v>
+        <v>55.870498547441031</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>
@@ -174,7 +174,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>37.668658374354713</v>
+        <v>33.73868240861232</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>11</v>
@@ -185,7 +185,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>10.563180831154085</v>
+        <v>14.639264531641869</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>11</v>
@@ -196,7 +196,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>44.772509396653362</v>
+        <v>38.083375505035008</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>11</v>
@@ -207,7 +207,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>36.672671170432999</v>
+        <v>15.681388231401629</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Turned all parsim into functions
</commit_message>
<xml_diff>
--- a/Graphs/normal flow rate details.xlsx
+++ b/Graphs/normal flow rate details.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="646" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="703" uniqueCount="15">
   <si>
     <t>normal_flow_rate_details1</t>
   </si>
@@ -109,9 +109,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="true"/>
-    <col min="2" max="2" width="14.5703125" customWidth="true"/>
-    <col min="3" max="3" width="4.85546875" customWidth="true"/>
+    <col min="1" max="1" width="24" customWidth="true"/>
+    <col min="2" max="2" width="13.46484375" customWidth="true"/>
+    <col min="3" max="3" width="4.73046875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -130,7 +130,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>54.473378555443993</v>
+        <v>54.951144613083095</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>11</v>
@@ -141,7 +141,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>32.598269851519511</v>
+        <v>26.309799551422486</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>11</v>
@@ -152,7 +152,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>13.411851961272751</v>
+        <v>18.404036144300758</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
@@ -163,7 +163,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>55.870498547441031</v>
+        <v>45.598273085931588</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>
@@ -174,7 +174,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>33.73868240861232</v>
+        <v>35.846945556233649</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>11</v>
@@ -185,7 +185,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>14.639264531641869</v>
+        <v>12.194011847007653</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>11</v>
@@ -196,7 +196,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>38.083375505035008</v>
+        <v>40.594365598338776</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>11</v>
@@ -207,7 +207,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>15.681388231401629</v>
+        <v>16.556238448663667</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
See if this works
</commit_message>
<xml_diff>
--- a/Graphs/normal flow rate details.xlsx
+++ b/Graphs/normal flow rate details.xlsx
@@ -13,9 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="950" uniqueCount="15">
-  <si>
-    <t>normal_flow_rate_details1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="76" uniqueCount="12">
+  <si>
+    <t>Operation phase</t>
   </si>
   <si>
     <t>Warm tank refuel chilldown</t>
@@ -42,22 +42,13 @@
     <t>Defuel wamrup</t>
   </si>
   <si>
-    <t>normal_flow_rate_details2</t>
-  </si>
-  <si>
-    <t>normal_flow_rate_details3</t>
+    <t>Mean flow rate</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
   <si>
     <t>m/s</t>
-  </si>
-  <si>
-    <t>Operation phase</t>
-  </si>
-  <si>
-    <t>Mean flow rate</t>
-  </si>
-  <si>
-    <t>Unit</t>
   </si>
 </sst>
 </file>
@@ -116,13 +107,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -130,7 +121,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>54.260289763386183</v>
+        <v>21.509545652562473</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>11</v>
@@ -141,7 +132,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>32.560683678541416</v>
+        <v>5.4887138399957749</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>11</v>
@@ -152,7 +143,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>15.685015910083401</v>
+        <v>16.180644693854031</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
@@ -163,7 +154,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>45.083278531798399</v>
+        <v>22.37187719861836</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>
@@ -174,7 +165,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>33.713325436308381</v>
+        <v>4.9961956554845965</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>11</v>
@@ -185,7 +176,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>12.867763186257303</v>
+        <v>27.436120310086068</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>11</v>
@@ -196,7 +187,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>40.493377081668868</v>
+        <v>30.451713659305238</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>11</v>
@@ -207,7 +198,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>15.186340600886382</v>
+        <v>15.822140733987464</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Added simplify data to simOut
</commit_message>
<xml_diff>
--- a/Graphs/normal flow rate details.xlsx
+++ b/Graphs/normal flow rate details.xlsx
@@ -100,9 +100,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="true"/>
-    <col min="2" max="2" width="14.5703125" customWidth="true"/>
-    <col min="3" max="3" width="4.85546875" customWidth="true"/>
+    <col min="1" max="1" width="24" customWidth="true"/>
+    <col min="2" max="2" width="13.46484375" customWidth="true"/>
+    <col min="3" max="3" width="4.73046875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -121,7 +121,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>33.715737664422008</v>
+        <v>29.953821277005368</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>11</v>
@@ -132,7 +132,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>2.8643075125809778</v>
+        <v>2.8282432808873317</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>11</v>
@@ -143,7 +143,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>17.672946448842847</v>
+        <v>42.331879980233133</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
@@ -154,7 +154,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>46.868462385135516</v>
+        <v>24.850481699987352</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>
@@ -165,7 +165,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>10.836205237344824</v>
+        <v>5.2102380718459118</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>11</v>
@@ -176,7 +176,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>17.843623424291518</v>
+        <v>41.76100252053034</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>11</v>
@@ -187,7 +187,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>30.488507146666773</v>
+        <v>29.441554371981745</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>11</v>
@@ -198,7 +198,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>15.695620009799692</v>
+        <v>30.693010113113001</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Added save file flag
</commit_message>
<xml_diff>
--- a/Graphs/normal flow rate details.xlsx
+++ b/Graphs/normal flow rate details.xlsx
@@ -100,9 +100,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="true"/>
-    <col min="2" max="2" width="14.5703125" customWidth="true"/>
-    <col min="3" max="3" width="4.85546875" customWidth="true"/>
+    <col min="1" max="1" width="24" customWidth="true"/>
+    <col min="2" max="2" width="13.46484375" customWidth="true"/>
+    <col min="3" max="3" width="4.73046875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -121,7 +121,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>29.964160680031473</v>
+        <v>29.953821277005368</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>11</v>
@@ -132,7 +132,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>2.8162993626697821</v>
+        <v>2.8282432808873317</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>11</v>
@@ -143,7 +143,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>42.322612779287027</v>
+        <v>42.331879980233133</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
@@ -154,7 +154,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>24.623276555115901</v>
+        <v>24.850481699987352</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>
@@ -165,7 +165,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>5.1952042446148887</v>
+        <v>5.2102380718459118</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>11</v>
@@ -176,7 +176,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>41.823153341390359</v>
+        <v>41.76100252053034</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>11</v>
@@ -187,7 +187,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>29.437629755248917</v>
+        <v>29.441554371981745</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>11</v>
@@ -198,7 +198,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>30.649747510032938</v>
+        <v>30.693010113113001</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>11</v>

</xml_diff>